<commit_message>
elozo orak plusz eheti 11c done
</commit_message>
<xml_diff>
--- a/10b/10_2024_03_07/ora.xlsx
+++ b/10b/10_2024_03_07/ora.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\palyi\bullshitBundle\kossuth\10b\10_2024_03_07\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\palyi\OneDrive\Desktop\bullshitBundle\kossuthrepo\10b\10_2024_03_07\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7776B26C-9C69-4115-A700-EF577DD36B31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{208841CA-0CEB-49D8-8DC4-065E74CA32AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F2892D76-E608-47D8-A275-EA75549DB126}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{F2892D76-E608-47D8-A275-EA75549DB126}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -750,7 +750,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -4611,19 +4611,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16E35CED-89F3-49E0-B0D7-1B355A0B5BED}">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D10" zoomScale="68" workbookViewId="0">
       <selection sqref="A1:C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.73046875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4634,7 +4634,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4645,7 +4645,7 @@
         <v>44941</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -4656,7 +4656,7 @@
         <v>44977</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -4667,7 +4667,7 @@
         <v>44995</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -4675,7 +4675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -4683,7 +4683,7 @@
         <v>450000</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -4691,7 +4691,7 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -4699,7 +4699,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -4707,7 +4707,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -4718,7 +4718,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -4729,7 +4729,7 @@
         <v>350000</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -4740,7 +4740,7 @@
         <v>380000</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -4751,7 +4751,7 @@
         <v>400000</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -4762,7 +4762,7 @@
         <v>420000</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -4773,7 +4773,7 @@
         <v>450000</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -4784,7 +4784,7 @@
         <v>470000</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -4795,7 +4795,7 @@
         <v>480000</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -4806,7 +4806,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -4817,7 +4817,7 @@
         <v>520000</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -4828,7 +4828,7 @@
         <v>550000</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -4839,7 +4839,7 @@
         <v>570000</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -4850,7 +4850,7 @@
         <v>600000</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -4861,7 +4861,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -4872,7 +4872,7 @@
         <v>1500000</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -4883,7 +4883,7 @@
         <v>900000</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -4894,7 +4894,7 @@
         <v>1200000</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>32</v>
       </c>

</xml_diff>